<commit_message>
Update product backlog concept
</commit_message>
<xml_diff>
--- a/Documenten/Concept Product Backlog.xlsx
+++ b/Documenten/Concept Product Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Prioriteit</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t xml:space="preserve">Ik wil de mogelijkheid om de gerechten te markeren als favoriet waar ik dan snel naar toe kan gaan via een favorieten lijst op de hoofdpagina. Dit wil ik om het gebruiksvriendelijker te maken. </t>
+  </si>
+  <si>
+    <t>Bewoners</t>
+  </si>
+  <si>
+    <t>Ik wil een veiligheidsknop die op elk moment te bereiken is die linkt naar een pagina met de meest voorkomende remedies tegen ongelukken. 1e hulp, wat te doen bij brand etc. Dit wil ik om de veiligheid te bevorderen.</t>
+  </si>
+  <si>
+    <t>Ik wil op elke stap van het koken een nuttige tip hebben die de veiligheid en / of efficientie van het koken bevorderd, denk hierbij aan natte doek onder de snijplank om weg glijden te voorkomen etc. Dit wil ik om de veiligheid te bevorderen.</t>
   </si>
 </sst>
 </file>
@@ -439,16 +448,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="210.42578125" customWidth="1"/>
+    <col min="5" max="5" width="214.28515625" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -670,6 +679,35 @@
       </c>
       <c r="E15" s="2" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>